<commit_message>
revision path excel for data center
</commit_message>
<xml_diff>
--- a/src/testdata/LoginForm.xlsx
+++ b/src/testdata/LoginForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\e-commerceTesting\src\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\eCommerceTEsting_automationexercise.com\src\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F6D4F0-6FEA-492F-A8E3-E3FD51683F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91C7466-6FC5-4155-AD46-4B67BF6DA135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="1850" windowWidth="11840" windowHeight="7270" xr2:uid="{35546CC2-1C8B-462C-ABCA-2121C1C6DB80}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{35546CC2-1C8B-462C-ABCA-2121C1C6DB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -34,9 +34,6 @@
     <t>kukuhpradipto@gmail.com</t>
   </si>
   <si>
-    <t>Kukuh1998</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -44,13 +41,25 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>Kukuh1</t>
+  </si>
+  <si>
+    <t>kukuhpradipto1@gmail.com</t>
+  </si>
+  <si>
+    <t>Kukuh2</t>
+  </si>
+  <si>
+    <t>kukuhpradipto2@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +71,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,9 +103,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -411,7 +425,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -422,33 +436,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{334F0D11-F956-4AB8-B1AF-744AB7A87D55}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{B36E37CE-2D91-45F4-B6FE-32182DFB9AB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -464,41 +488,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="23.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>